<commit_message>
feat: Complete CBIC implementation and architecture transition prep
- Added comprehensive CBIC data functions (cement, steel, PIM)
- Removed renv dependency management
- Updated CLAUDE.md with new architecture plans (3-phase transition)
- Added .gitignore entries for claude/ and .DS_Store files
- Updated .Rbuildignore for package building
- Prepared for migration to unified data interface (list_datasets/get_dataset)

This commit combines the completed CBIC work with preparation for the new
architecture that will provide a simpler, more robust data distribution system.
</commit_message>
<xml_diff>
--- a/data-raw/bacen_codes.xlsx
+++ b/data-raw/bacen_codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciusoike/Documents/GitHub/realestatebr/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciusreginatto/GitHub/realestatebr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7DB851-34FE-914B-812C-B395317816F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48242F5D-BEDE-3F44-ABBD-8C3784E5717D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="1320" windowWidth="28800" windowHeight="15760" xr2:uid="{0BDEE7C6-332B-4F5C-8740-144CDD417F7B}"/>
+    <workbookView xWindow="1440" yWindow="1240" windowWidth="28800" windowHeight="15760" xr2:uid="{0BDEE7C6-332B-4F5C-8740-144CDD417F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -1451,9 +1451,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1491,7 +1491,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1597,7 +1597,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1739,7 +1739,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1749,7 +1749,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174ADDEC-0EF3-47A4-873A-4CADD97CAD34}">
   <dimension ref="A1:H141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1757,7 +1759,9 @@
     <col min="2" max="2" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="108.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
@@ -2545,7 +2549,7 @@
         <v>4466</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>278</v>

</xml_diff>

<commit_message>
fix: Resolve package check warnings and documentation issues
- Fix missing dependencies: Add geobr, sf, stringi to DESCRIPTION Imports
- Fix Rd file Unicode warnings: Replace non-ASCII characters with ASCII equivalents in roxygen comments
- Update .Rbuildignore: Add comprehensive patterns for development files to reduce top-level files NOTE
- Replace Unicode escapes in documentation:
  * get_fgv_indicators.R: "Getúlio" → "Getulio"
  * get_rppi.R: "Índice", "Imóveis", "São Paulo", "Seminário" → ASCII equivalents
  * get_cbic.R: "aço" → "aco" in function examples
- Regenerate all Rd documentation files with devtools::document()

Resolves: R CMD check warnings for Rd files and missing dependencies
Improves: Package compliance and reduces NOTEs for CRAN submission

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data-raw/bacen_codes.xlsx
+++ b/data-raw/bacen_codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciusoike/Documents/GitHub/realestatebr/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciusreginatto/GitHub/realestatebr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7DB851-34FE-914B-812C-B395317816F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD522752-591C-6346-AF8B-EF87094BB3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="1320" windowWidth="28800" windowHeight="15760" xr2:uid="{0BDEE7C6-332B-4F5C-8740-144CDD417F7B}"/>
+    <workbookView xWindow="1440" yWindow="1320" windowWidth="28800" windowHeight="15760" xr2:uid="{0BDEE7C6-332B-4F5C-8740-144CDD417F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -1451,9 +1451,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1491,7 +1491,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1597,7 +1597,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1739,7 +1739,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1747,9 +1747,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174ADDEC-0EF3-47A4-873A-4CADD97CAD34}">
-  <dimension ref="A1:H141"/>
+  <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1760,7 +1762,7 @@
     <col min="5" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>200</v>
       </c>
@@ -1780,7 +1782,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>189</v>
       </c>
@@ -1800,7 +1802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>190</v>
       </c>
@@ -1819,8 +1821,11 @@
       <c r="F3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="L3" s="5">
+        <v>20704</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="5">
         <v>192</v>
       </c>
@@ -1839,8 +1844,11 @@
       <c r="F4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="L4" s="1">
+        <v>20756</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="5">
         <v>432</v>
       </c>
@@ -1859,8 +1867,11 @@
       <c r="F5" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="L5" s="1">
+        <v>20768</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="5">
         <v>433</v>
       </c>
@@ -1879,8 +1890,11 @@
       <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="L6" s="5">
+        <v>20914</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
         <v>606</v>
       </c>
@@ -1899,8 +1913,11 @@
       <c r="F7" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="L7" s="1">
+        <v>21072</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="5">
         <v>619</v>
       </c>
@@ -1919,8 +1936,11 @@
       <c r="F8" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="L8" s="5">
+        <v>21084</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="5">
         <v>632</v>
       </c>
@@ -1939,8 +1959,11 @@
       <c r="F9" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="L9" s="5">
+        <v>21340</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10" s="5">
         <v>645</v>
       </c>
@@ -1959,8 +1982,11 @@
       <c r="F10" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="L10" s="5">
+        <v>24364</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11" s="5">
         <v>918</v>
       </c>
@@ -1979,8 +2005,11 @@
       <c r="F11" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="L11" s="5">
+        <v>28545</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" s="5">
         <v>931</v>
       </c>
@@ -1999,8 +2028,11 @@
       <c r="F12" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="L12" s="5">
+        <v>28763</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" s="5">
         <v>944</v>
       </c>
@@ -2019,8 +2051,11 @@
       <c r="F13" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="L13" s="5">
+        <v>28770</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14" s="5">
         <v>957</v>
       </c>
@@ -2040,7 +2075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <v>1344</v>
       </c>
@@ -2060,7 +2095,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <v>1346</v>
       </c>

</xml_diff>